<commit_message>
model training process is completed
</commit_message>
<xml_diff>
--- a/data/training_validation_logs.xlsx
+++ b/data/training_validation_logs.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -493,7 +493,7 @@
       </c>
       <c r="B2" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C2" s="3" t="inlineStr">
@@ -523,7 +523,7 @@
       </c>
       <c r="B3" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C3" s="3" t="inlineStr">
@@ -553,7 +553,7 @@
       </c>
       <c r="B4" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C4" s="3" t="inlineStr">
@@ -583,7 +583,7 @@
       </c>
       <c r="B5" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C5" s="3" t="inlineStr">
@@ -613,7 +613,7 @@
       </c>
       <c r="B6" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C6" s="3" t="inlineStr">
@@ -643,7 +643,7 @@
       </c>
       <c r="B7" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C7" s="3" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="B8" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C8" s="3" t="inlineStr">
@@ -703,7 +703,7 @@
       </c>
       <c r="B9" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C9" s="3" t="inlineStr">
@@ -733,7 +733,7 @@
       </c>
       <c r="B10" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C10" s="3" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="B11" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C11" s="3" t="inlineStr">
@@ -793,7 +793,7 @@
       </c>
       <c r="B12" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C12" s="3" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="B13" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
@@ -853,7 +853,7 @@
       </c>
       <c r="B14" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
@@ -883,7 +883,7 @@
       </c>
       <c r="B15" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C15" s="3" t="inlineStr">
@@ -913,7 +913,7 @@
       </c>
       <c r="B16" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C16" s="3" t="inlineStr">
@@ -943,7 +943,7 @@
       </c>
       <c r="B17" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C17" s="3" t="inlineStr">
@@ -973,7 +973,7 @@
       </c>
       <c r="B18" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C18" s="3" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="B19" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C19" s="3" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B20" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
@@ -1063,7 +1063,7 @@
       </c>
       <c r="B21" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C21" s="3" t="inlineStr">
@@ -1093,7 +1093,7 @@
       </c>
       <c r="B22" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C22" s="3" t="inlineStr">
@@ -1123,7 +1123,7 @@
       </c>
       <c r="B23" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
@@ -1153,7 +1153,7 @@
       </c>
       <c r="B24" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C24" s="3" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="B25" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C25" s="3" t="inlineStr">
@@ -1213,7 +1213,7 @@
       </c>
       <c r="B26" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C26" s="3" t="inlineStr">
@@ -1243,7 +1243,7 @@
       </c>
       <c r="B27" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
@@ -1273,7 +1273,7 @@
       </c>
       <c r="B28" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
@@ -1303,7 +1303,7 @@
       </c>
       <c r="B29" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
@@ -1333,7 +1333,7 @@
       </c>
       <c r="B30" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C30" s="3" t="inlineStr">
@@ -1363,7 +1363,7 @@
       </c>
       <c r="B31" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C31" s="3" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="B32" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
@@ -1423,7 +1423,7 @@
       </c>
       <c r="B33" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C33" s="3" t="inlineStr">
@@ -1453,7 +1453,7 @@
       </c>
       <c r="B34" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C34" s="3" t="inlineStr">
@@ -1483,7 +1483,7 @@
       </c>
       <c r="B35" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C35" s="3" t="inlineStr">
@@ -1513,7 +1513,7 @@
       </c>
       <c r="B36" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
@@ -1543,7 +1543,7 @@
       </c>
       <c r="B37" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
@@ -1573,7 +1573,7 @@
       </c>
       <c r="B38" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
@@ -1603,7 +1603,7 @@
       </c>
       <c r="B39" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
@@ -1633,7 +1633,7 @@
       </c>
       <c r="B40" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="B41" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C41" s="3" t="inlineStr">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B42" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C42" s="3" t="inlineStr">
@@ -1723,7 +1723,7 @@
       </c>
       <c r="B43" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
@@ -1753,7 +1753,7 @@
       </c>
       <c r="B44" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B45" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="B46" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B47" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="B48" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
@@ -1903,7 +1903,7 @@
       </c>
       <c r="B49" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
@@ -1933,7 +1933,7 @@
       </c>
       <c r="B50" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C50" s="3" t="inlineStr">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B51" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C51" s="3" t="inlineStr">
@@ -1993,7 +1993,7 @@
       </c>
       <c r="B52" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C52" s="3" t="inlineStr">
@@ -2023,7 +2023,7 @@
       </c>
       <c r="B53" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C53" s="3" t="inlineStr">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="B54" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C54" s="3" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="B55" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C55" s="3" t="inlineStr">
@@ -2113,7 +2113,7 @@
       </c>
       <c r="B56" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C56" s="3" t="inlineStr">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="B57" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C57" s="3" t="inlineStr">
@@ -2173,7 +2173,7 @@
       </c>
       <c r="B58" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C58" s="3" t="inlineStr">
@@ -2203,7 +2203,7 @@
       </c>
       <c r="B59" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C59" s="3" t="inlineStr">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B60" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C60" s="3" t="inlineStr">
@@ -2263,7 +2263,7 @@
       </c>
       <c r="B61" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C61" s="3" t="inlineStr">
@@ -2293,7 +2293,7 @@
       </c>
       <c r="B62" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C62" s="3" t="inlineStr">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B63" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C63" s="3" t="inlineStr">
@@ -2353,7 +2353,7 @@
       </c>
       <c r="B64" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C64" s="3" t="inlineStr">
@@ -2383,7 +2383,7 @@
       </c>
       <c r="B65" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C65" s="3" t="inlineStr">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B66" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C66" s="3" t="inlineStr">
@@ -2443,7 +2443,7 @@
       </c>
       <c r="B67" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C67" s="3" t="inlineStr">
@@ -2473,7 +2473,7 @@
       </c>
       <c r="B68" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C68" s="3" t="inlineStr">
@@ -2503,7 +2503,7 @@
       </c>
       <c r="B69" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C69" s="3" t="inlineStr">
@@ -2533,7 +2533,7 @@
       </c>
       <c r="B70" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C70" s="3" t="inlineStr">
@@ -2563,7 +2563,7 @@
       </c>
       <c r="B71" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C71" s="3" t="inlineStr">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="B72" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C72" s="3" t="inlineStr">
@@ -2623,7 +2623,7 @@
       </c>
       <c r="B73" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C73" s="3" t="inlineStr">
@@ -2653,7 +2653,7 @@
       </c>
       <c r="B74" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C74" s="3" t="inlineStr">
@@ -2683,7 +2683,7 @@
       </c>
       <c r="B75" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C75" s="3" t="inlineStr">
@@ -2713,7 +2713,7 @@
       </c>
       <c r="B76" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C76" s="3" t="inlineStr">
@@ -2743,7 +2743,7 @@
       </c>
       <c r="B77" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C77" s="3" t="inlineStr">
@@ -2773,7 +2773,7 @@
       </c>
       <c r="B78" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C78" s="3" t="inlineStr">
@@ -2803,7 +2803,7 @@
       </c>
       <c r="B79" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C79" s="3" t="inlineStr">
@@ -2833,7 +2833,7 @@
       </c>
       <c r="B80" s="3" t="inlineStr">
         <is>
-          <t>2024-09-16</t>
+          <t>2024-09-17</t>
         </is>
       </c>
       <c r="C80" s="3" t="inlineStr">

</xml_diff>